<commit_message>
Add cluster, organisations, admin1
</commit_message>
<xml_diff>
--- a/html/modules/custom/ocha_assessments/bulk_template.xlsx
+++ b/html/modules/custom/ocha_assessments/bulk_template.xlsx
@@ -5,13 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Accessibility" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Status" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PopulationTypes" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Clusters" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Organizations" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Admin1" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +26,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+  <si>
+    <t xml:space="preserve">Assessment Registry – </t>
+  </si>
   <si>
     <r>
       <rPr>
@@ -63,6 +69,35 @@
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF003366"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Mandatory fields are marked with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF003366"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -565,7 +600,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -626,6 +661,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF003366"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF003366"/>
@@ -650,19 +697,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -777,10 +817,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,11 +836,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,31 +852,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -860,10 +900,10 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.52"/>
   </cols>
@@ -873,12 +913,21 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -903,14 +952,16 @@
       <c r="X3" s="6"/>
     </row>
     <row r="4" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="5"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -927,16 +978,16 @@
       <c r="X4" s="6"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="s">
-        <v>1</v>
-      </c>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="3"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -945,41 +996,41 @@
     </row>
     <row r="6" s="2" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -988,157 +1039,158 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
       <c r="V6" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
     </row>
     <row r="7" s="2" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T7" s="13"/>
       <c r="U7" s="16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="V7" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W7" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X7" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="true" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="U8" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="V8" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="X8" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C3:J4"/>
-    <mergeCell ref="D5:H5"/>
+  <mergeCells count="10">
+    <mergeCell ref="C2:J3"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:J5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="O6:U6"/>
@@ -1190,29 +1242,29 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="18.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1237,31 +1289,31 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1282,11 +1334,11 @@
   </sheetPr>
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22"/>
@@ -1378,4 +1430,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add admin levels and more
</commit_message>
<xml_diff>
--- a/html/modules/custom/ocha_assessments/bulk_template.xlsx
+++ b/html/modules/custom/ocha_assessments/bulk_template.xlsx
@@ -5,16 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Assessments" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Accessibility" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Status" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="PopulationTypes" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Clusters" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Organizations" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Admin1" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Units" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CollectionMethod" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PopulationTypes" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Clusters" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Organizations" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="AdminLevel1" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="AdminLevel2" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="AdminLevel3" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t xml:space="preserve">Assessment Registry – </t>
   </si>
@@ -80,6 +84,7 @@
         <color rgb="FF003366"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Mandatory fields are marked with </t>
     </r>
@@ -89,6 +94,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">*</t>
     </r>
@@ -98,6 +104,7 @@
         <color rgb="FF003366"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -370,7 +377,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Kebele/ Town/ Other</t>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <r>
@@ -590,6 +597,48 @@
   </si>
   <si>
     <t xml:space="preserve">Report completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settlements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Households</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structured Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unstructured Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Informant Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focus group discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline data analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email / Mail Interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixed</t>
   </si>
 </sst>
 </file>
@@ -665,12 +714,14 @@
       <color rgb="FF003366"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -816,11 +867,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -899,11 +950,11 @@
   </sheetPr>
   <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.52"/>
   </cols>
@@ -1199,7 +1250,7 @@
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="7">
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="Q1:Q8" type="list">
       <formula1>Accessibility!$A$1:$A$4</formula1>
       <formula2>0</formula2>
@@ -1220,10 +1271,64 @@
       <formula1>PopulationTypes!$A$1:$A$43</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M9" type="list">
+      <formula1>Units!$A$1:$A$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N9" type="list">
+      <formula1>CollectionMethod!$A$1:$A$16</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1242,7 +1347,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="18.66"/>
   </cols>
@@ -1289,7 +1394,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
@@ -1332,94 +1437,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22"/>
+      <c r="A1" s="22" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
+      <c r="A2" s="22" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22"/>
+      <c r="A3" s="22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22"/>
+      <c r="A4" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1437,14 +1481,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1460,14 +1560,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1485,11 +1667,57 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add Id to template creator, limit cluster by operation
</commit_message>
<xml_diff>
--- a/html/modules/custom/ocha_assessments/bulk_template.xlsx
+++ b/html/modules/custom/ocha_assessments/bulk_template.xlsx
@@ -951,11 +951,19 @@
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1301,7 +1309,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1324,7 +1332,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1347,7 +1355,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="18.66"/>
   </cols>
@@ -1394,7 +1402,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
@@ -1443,7 +1451,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
@@ -1487,7 +1495,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
@@ -1566,7 +1574,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22"/>
@@ -1671,7 +1679,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1694,7 +1702,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1717,7 +1725,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>